<commit_message>
update zone track & zone
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\WellInsight\wi-angular\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="171027" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
   <si>
     <t>Code</t>
   </si>
@@ -256,9 +261,6 @@
     <t>New Track</t>
   </si>
   <si>
-    <t>Duplicate Track</t>
-  </si>
-  <si>
     <t>Delete Track</t>
   </si>
   <si>
@@ -443,12 +445,24 @@
   </si>
   <si>
     <t xml:space="preserve">Range Specific </t>
+  </si>
+  <si>
+    <t>Duplicate Log Track</t>
+  </si>
+  <si>
+    <t>zonation_track_add_16x16</t>
+  </si>
+  <si>
+    <t>Add Zonation Track</t>
+  </si>
+  <si>
+    <t>AddZonationTrackButton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -538,6 +552,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -798,18 +815,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -857,10 +874,10 @@
         <v>12</v>
       </c>
       <c r="K1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -901,7 +918,7 @@
         <v>Button</v>
       </c>
       <c r="E3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
@@ -932,7 +949,7 @@
         <v>51</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ref="F4:F46" si="0">SUBSTITUTE(E4,"_","-")</f>
+        <f t="shared" ref="F4:F47" si="0">SUBSTITUTE(E4,"_","-")</f>
         <v>save-16x16</v>
       </c>
       <c r="J4" t="s">
@@ -1013,7 +1030,7 @@
         <v>Button</v>
       </c>
       <c r="E7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -1028,22 +1045,22 @@
     </row>
     <row r="8" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>54</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>13</v>
@@ -1054,278 +1071,278 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
         <v>93</v>
       </c>
-      <c r="B9" t="s">
-        <v>94</v>
-      </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" t="s">
+        <v>136</v>
+      </c>
+      <c r="L9" t="s">
         <v>137</v>
-      </c>
-      <c r="L9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H10" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" t="s">
         <v>137</v>
-      </c>
-      <c r="L10" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
+        <v>136</v>
+      </c>
+      <c r="L11" t="s">
         <v>137</v>
-      </c>
-      <c r="L11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" t="s">
         <v>137</v>
-      </c>
-      <c r="L12" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L13" t="s">
         <v>137</v>
-      </c>
-      <c r="L13" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L14" t="s">
         <v>137</v>
-      </c>
-      <c r="L14" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H15" t="s">
+        <v>136</v>
+      </c>
+      <c r="L15" t="s">
         <v>137</v>
-      </c>
-      <c r="L15" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" t="s">
+        <v>136</v>
+      </c>
+      <c r="L16" t="s">
         <v>137</v>
-      </c>
-      <c r="L16" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
+        <v>136</v>
+      </c>
+      <c r="L17" t="s">
         <v>137</v>
-      </c>
-      <c r="L17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H18" t="s">
+        <v>136</v>
+      </c>
+      <c r="L18" t="s">
         <v>137</v>
-      </c>
-      <c r="L18" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H19" t="s">
+        <v>136</v>
+      </c>
+      <c r="L19" t="s">
         <v>137</v>
-      </c>
-      <c r="L19" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" t="s">
         <v>137</v>
-      </c>
-      <c r="L20" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1376,7 +1393,7 @@
         <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1404,7 +1421,7 @@
         <v>13</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1441,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="D25" t="str">
-        <f t="shared" ref="D25:D32" si="2">REPLACE(C25, 1, 2, "")</f>
+        <f t="shared" ref="D25:D33" si="2">REPLACE(C25, 1, 2, "")</f>
         <v>Button</v>
       </c>
       <c r="E25" t="s">
@@ -1463,7 +1480,7 @@
         <v>3.2</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>7</v>
@@ -1483,7 +1500,7 @@
         <v>13</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1552,7 +1569,7 @@
         <v>Button</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F29" t="str">
         <f>SUBSTITUTE(E29,"_","-")</f>
@@ -1618,7 +1635,7 @@
         <v>13</v>
       </c>
       <c r="K31" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1626,356 +1643,362 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" ref="D32" si="3">REPLACE(C32, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" ref="F32" si="4">SUBSTITUTE(E32,"_","-")</f>
+        <v>zonation-track-add-16x16</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="str">
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>60</v>
       </c>
-      <c r="F32" t="str">
+      <c r="F33" t="str">
         <f t="shared" si="0"/>
         <v>track-delete-16x16</v>
       </c>
-      <c r="J32" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
+      <c r="J33" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>5</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="1" t="str">
-        <f t="shared" ref="D33:D46" si="3">REPLACE(C33, 1, 2, "")</f>
+      <c r="D34" s="1" t="str">
+        <f t="shared" ref="D34:D47" si="5">REPLACE(C34, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="3"/>
-        <v>Button</v>
-      </c>
-      <c r="E34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v>marker-add-16x16</v>
-      </c>
-      <c r="J34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" t="s">
-        <v>80</v>
-      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>zone-edit-16x16</v>
+        <v>marker-add-16x16</v>
       </c>
       <c r="J35" t="s">
         <v>13</v>
       </c>
       <c r="K35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>annotation-16x16</v>
+        <v>zone-edit-16x16</v>
       </c>
       <c r="J36" t="s">
         <v>13</v>
       </c>
       <c r="K36" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>5.4</v>
+        <v>5.3</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>image-add-16x16</v>
+        <v>annotation-16x16</v>
       </c>
       <c r="J37" t="s">
         <v>13</v>
       </c>
       <c r="K37" t="s">
-        <v>82</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>5.5</v>
+        <v>5.4</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Button</v>
       </c>
       <c r="E38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>shading-add-16x16</v>
+        <v>image-add-16x16</v>
       </c>
       <c r="J38" t="s">
         <v>13</v>
       </c>
       <c r="K38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="5"/>
+        <v>Button</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>shading-add-16x16</v>
+      </c>
+      <c r="J39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
         <v>5.6</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>41</v>
       </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="3"/>
-        <v>Button</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="5"/>
+        <v>Button</v>
+      </c>
+      <c r="E40" t="s">
         <v>66</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F40" t="str">
         <f t="shared" si="0"/>
         <v>visual-remove-16x16</v>
       </c>
-      <c r="J39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="J40" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
         <v>6</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D41" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>6.1</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="3"/>
-        <v>Button</v>
-      </c>
-      <c r="E41" t="s">
-        <v>67</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="0"/>
-        <v>crossplot-new-16x16</v>
-      </c>
-      <c r="J41" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" t="s">
-        <v>85</v>
-      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
+        <v>6.1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="5"/>
+        <v>Button</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>crossplot-new-16x16</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
         <v>6.2</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="3"/>
-        <v>Button</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="5"/>
+        <v>Button</v>
+      </c>
+      <c r="E43" t="s">
         <v>68</v>
       </c>
-      <c r="F42" t="str">
+      <c r="F43" t="str">
         <f t="shared" si="0"/>
         <v>histogram-new-16x16</v>
       </c>
-      <c r="J42" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="1" t="str">
-        <f t="shared" si="3"/>
+      <c r="D44" s="1" t="str">
+        <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>7.1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="3"/>
-        <v>Checkbox</v>
-      </c>
-      <c r="F44" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G44" t="s">
-        <v>88</v>
-      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
         <v>48</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Checkbox</v>
       </c>
       <c r="F45" t="str">
@@ -1983,21 +2006,21 @@
         <v/>
       </c>
       <c r="G45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>Checkbox</v>
       </c>
       <c r="F46" t="str">
@@ -2005,7 +2028,29 @@
         <v/>
       </c>
       <c r="G46" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>7.3</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="5"/>
+        <v>Checkbox</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G47" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2015,7 +2060,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update image log track
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
   <si>
     <t>Code</t>
   </si>
@@ -448,13 +448,29 @@
   </si>
   <si>
     <t>AddZonationTrackButton</t>
+  </si>
+  <si>
+    <t>RemoveImageButton</t>
+  </si>
+  <si>
+    <t>image_delete_16x16</t>
+  </si>
+  <si>
+    <t>Remove Image</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -501,34 +517,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,1206 +830,1236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="11" style="2"/>
+    <col min="10" max="10" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="str">
+      <c r="D2" s="4" t="str">
         <f>REPLACE(C2, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="str">
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="str">
         <f>REPLACE(C3, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F3" s="2" t="str">
         <f>SUBSTITUTE(E3,"_","-")</f>
         <v>properties-16x16</v>
       </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" s="1">
         <v>1.2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="str">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="str">
         <f>REPLACE(C4, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" ref="F4:F46" si="0">SUBSTITUTE(E4,"_","-")</f>
+      <c r="F4" s="2" t="str">
+        <f t="shared" ref="F4:F47" si="0">SUBSTITUTE(E4,"_","-")</f>
         <v>save-16x16</v>
       </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="J4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A5" s="1">
         <v>1.3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="str">
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="str">
         <f t="shared" ref="D5:D7" si="1">REPLACE(C5, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F5" t="str">
+      <c r="F5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>save-as-16x16</v>
       </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A6" s="6">
         <v>1.4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="str">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Button</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F6" t="str">
+      <c r="F6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>print-16x16</v>
       </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A7" s="6">
         <v>1.5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="str">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f t="shared" si="1"/>
         <v>Button</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F7" t="str">
+      <c r="F7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>arrow-right-16x16</v>
       </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="9" t="s">
+      <c r="J8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A11" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A21" s="10">
         <v>2</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="1" t="str">
+      <c r="D21" s="4" t="str">
         <f>REPLACE(C21, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A22" s="11">
         <v>2.1</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="str">
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="2" t="str">
         <f>REPLACE(C22, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F22" t="str">
+      <c r="F22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zoom-in-16x16</v>
       </c>
-      <c r="J22" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="J22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A23" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="str">
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="2" t="str">
         <f>REPLACE(C23, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="str">
+      <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zoom-out-16x16</v>
       </c>
-      <c r="J23" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="J23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A24" s="10">
         <v>3</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="1" t="str">
+      <c r="D24" s="4" t="str">
         <f>REPLACE(C24, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A25" s="11">
         <v>3.1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="str">
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="str">
         <f t="shared" ref="D25:D33" si="2">REPLACE(C25, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F25" t="str">
+      <c r="F25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>plot-range-16x16</v>
       </c>
-      <c r="J25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="J25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+    <row r="26" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="12">
         <v>3.2</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="12" t="str">
+      <c r="C26" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="12" t="str">
+      <c r="F26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>plot-range-specific-16x16</v>
       </c>
-      <c r="J26" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="12" t="s">
+      <c r="J26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K26" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A27" s="11">
         <v>3.3</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="str">
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F27" t="str">
+      <c r="F27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>plot-whole-well-16x16</v>
       </c>
-      <c r="J27" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A28" s="10">
         <v>4</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="1" t="str">
+      <c r="D28" s="4" t="str">
         <f>REPLACE(C28, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A29" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="str">
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F29" s="2" t="str">
         <f>SUBSTITUTE(E29,"_","-")</f>
         <v>depth-axis-add-16x16</v>
       </c>
-      <c r="J29" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="J29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A30" s="11">
         <v>4.2</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="str">
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>logplot-new-16x16</v>
       </c>
-      <c r="J30" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="J30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A31" s="11">
         <v>4.3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="str">
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F31" t="str">
+      <c r="F31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>track-duplicate-16x16</v>
       </c>
-      <c r="J31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="J31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A32" s="11">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="str">
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2" t="str">
         <f t="shared" ref="D32" si="3">REPLACE(C32, 1, 2, "")</f>
         <v>Button</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="F32" t="str">
+      <c r="F32" s="2" t="str">
         <f t="shared" ref="F32" si="4">SUBSTITUTE(E32,"_","-")</f>
         <v>zonation-track-add-16x16</v>
       </c>
-      <c r="J32" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="J32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A33" s="11">
         <v>4.5</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="str">
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F33" t="str">
+      <c r="F33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>track-delete-16x16</v>
       </c>
-      <c r="J33" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="J33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A34" s="10">
         <v>5</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="1" t="str">
-        <f t="shared" ref="D34:D46" si="5">REPLACE(C34, 1, 2, "")</f>
+      <c r="D34" s="4" t="str">
+        <f t="shared" ref="D34:D47" si="5">REPLACE(C34, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A35" s="11">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="str">
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F35" t="str">
+      <c r="F35" s="2" t="str">
         <f t="shared" si="0"/>
         <v>marker-add-16x16</v>
       </c>
-      <c r="J35" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="J35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A36" s="11">
         <v>5.2</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" t="str">
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F36" t="str">
+      <c r="F36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zone-edit-16x16</v>
       </c>
-      <c r="J36" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" t="s">
+      <c r="J36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A37" s="11">
         <v>5.3</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="str">
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F37" t="str">
+      <c r="F37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>annotation-16x16</v>
       </c>
-      <c r="J37" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" t="s">
+      <c r="J37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A38" s="11">
         <v>5.4</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" t="str">
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2" t="str">
+        <f t="shared" ref="D38" si="6">REPLACE(C38, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="2" t="str">
+        <f t="shared" ref="F38" si="7">SUBSTITUTE(E38,"_","-")</f>
+        <v>image-add-16x16</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A39" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E38" t="s">
-        <v>63</v>
-      </c>
-      <c r="F38" t="str">
+      <c r="E39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>image-add-16x16</v>
-      </c>
-      <c r="J38" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>5.5</v>
-      </c>
-      <c r="B39" t="s">
+        <v>image-delete-16x16</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A40" s="11">
+        <v>5.6</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="str">
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F39" t="str">
+      <c r="F40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>shading-add-16x16</v>
       </c>
-      <c r="J39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="J40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A41" s="10">
         <v>6</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="1" t="str">
+      <c r="D41" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A42" s="11">
         <v>6.1</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="str">
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F41" t="str">
+      <c r="F42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>crossplot-new-16x16</v>
       </c>
-      <c r="J41" t="s">
-        <v>13</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="J42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A43" s="11">
         <v>6.2</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="str">
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F42" t="str">
+      <c r="F43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>histogram-new-16x16</v>
       </c>
-      <c r="J42" t="s">
-        <v>13</v>
-      </c>
-      <c r="K42" t="s">
+      <c r="J43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="6">
-        <v>7</v>
-      </c>
-      <c r="B43" s="1" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A44" s="10">
+        <v>7</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="1" t="str">
+      <c r="D44" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A45" s="11">
         <v>7.1</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D44" t="str">
+      <c r="D45" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Checkbox</v>
       </c>
-      <c r="F44" t="str">
+      <c r="F45" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A46" s="11">
         <v>7.2</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D45" t="str">
+      <c r="D46" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Checkbox</v>
       </c>
-      <c r="F45" t="str">
+      <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A47" s="11">
         <v>7.3</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D46" t="str">
+      <c r="D47" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Checkbox</v>
       </c>
-      <c r="F46" t="str">
+      <c r="F47" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G46" t="s">
+      <c r="G47" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2023,14 +2070,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add custom sacle to log-track
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\WellInsight\wi-angular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Github\wi-angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2076E37F-7BC3-4BDA-AC1B-8363A6788BD5}" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171026" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="147">
   <si>
     <t>Code</t>
   </si>
@@ -458,13 +457,22 @@
   </si>
   <si>
     <t>Tool tip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         1.6.13</t>
+  </si>
+  <si>
+    <t>ScaleCustomButton</t>
+  </si>
+  <si>
+    <t>Custom Scale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -518,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -547,12 +555,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFE4A506"/>
@@ -831,14 +868,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.375" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.75" style="2" bestFit="1" customWidth="1"/>
@@ -853,7 +890,7 @@
     <col min="12" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -891,7 +928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -914,7 +951,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -942,7 +979,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -960,7 +997,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" ref="F4:F47" si="0">SUBSTITUTE(E4,"_","-")</f>
+        <f t="shared" ref="F4:F48" si="0">SUBSTITUTE(E4,"_","-")</f>
         <v>save-16x16</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -970,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
@@ -998,7 +1035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1.4</v>
       </c>
@@ -1026,7 +1063,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1.5</v>
       </c>
@@ -1054,7 +1091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="8" customFormat="1">
+    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>31</v>
       </c>
@@ -1080,7 +1117,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1103,7 +1140,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -1126,7 +1163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -1149,7 +1186,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1172,7 +1209,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
@@ -1195,7 +1232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
@@ -1218,7 +1255,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -1241,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -1264,7 +1301,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -1287,7 +1324,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -1310,7 +1347,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -1333,7 +1370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>74</v>
       </c>
@@ -1356,249 +1393,244 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="10">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="4" t="str">
-        <f>REPLACE(C21, 1, 2, "")</f>
+      <c r="D22" s="4" t="str">
+        <f>REPLACE(C22, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11">
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
         <v>2.1</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="2" t="str">
-        <f>REPLACE(C22, 1, 2, "")</f>
-        <v>Button</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f>REPLACE(C23, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="2" t="str">
+      <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zoom-in-16x16</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="2" t="s">
+      <c r="J23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="11">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="2" t="str">
-        <f>REPLACE(C23, 1, 2, "")</f>
-        <v>Button</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f>REPLACE(C24, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="2" t="str">
+      <c r="F24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zoom-out-16x16</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="2" t="s">
+      <c r="J24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="10">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="4" t="str">
-        <f>REPLACE(C24, 1, 2, "")</f>
+      <c r="D25" s="4" t="str">
+        <f>REPLACE(C25, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="11">
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>3.1</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="2" t="str">
-        <f t="shared" ref="D25:D33" si="2">REPLACE(C25, 1, 2, "")</f>
-        <v>Button</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" ref="D26:D34" si="2">REPLACE(C26, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="2" t="str">
+      <c r="F26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>plot-range-16x16</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="2" t="s">
+      <c r="J26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="13" customFormat="1">
-      <c r="A26" s="12">
+    <row r="27" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12">
         <v>3.2</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="13" t="str">
+      <c r="C27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="13" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E27" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="13" t="str">
+      <c r="F27" s="13" t="str">
         <f t="shared" si="0"/>
         <v>plot-range-specific-16x16</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="13" t="s">
+      <c r="J27" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="11">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>3.3</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="2" t="str">
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="2" t="str">
+      <c r="F28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>plot-whole-well-16x16</v>
       </c>
-      <c r="J27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="2" t="s">
+      <c r="J28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="10">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>4</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="4" t="str">
-        <f>REPLACE(C28, 1, 2, "")</f>
+      <c r="D29" s="4" t="str">
+        <f>REPLACE(C29, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11">
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>Button</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="2" t="str">
-        <f>SUBSTITUTE(E29,"_","-")</f>
-        <v>depth-axis-add-16x16</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>15</v>
@@ -1608,424 +1640,430 @@
         <v>Button</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f>SUBSTITUTE(E30,"_","-")</f>
+        <v>depth-axis-add-16x16</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>4.2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Button</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="2" t="str">
+      <c r="F31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>logplot-new-16x16</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="2" t="s">
+      <c r="J31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="11">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>4.3</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="str">
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F31" s="2" t="str">
+      <c r="F32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>track-duplicate-16x16</v>
       </c>
-      <c r="J31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="2" t="s">
+      <c r="J32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="2" t="str">
-        <f t="shared" ref="D32" si="3">REPLACE(C32, 1, 2, "")</f>
-        <v>Button</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="2" t="str">
+        <f t="shared" ref="D33" si="3">REPLACE(C33, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="2" t="str">
-        <f t="shared" ref="F32" si="4">SUBSTITUTE(E32,"_","-")</f>
+      <c r="F33" s="2" t="str">
+        <f t="shared" ref="F33" si="4">SUBSTITUTE(E33,"_","-")</f>
         <v>zonation-track-add-16x16</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="2" t="s">
+      <c r="J33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="11">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>4.5</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="2" t="str">
+      <c r="C34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Button</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="2" t="str">
+      <c r="F34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>track-delete-16x16</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="2" t="s">
+      <c r="J34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="10">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>5</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="4" t="str">
-        <f t="shared" ref="D34:D47" si="5">REPLACE(C34, 1, 2, "")</f>
+      <c r="D35" s="4" t="str">
+        <f t="shared" ref="D35:D48" si="5">REPLACE(C35, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="11">
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="2" t="str">
+      <c r="C36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F35" s="2" t="str">
+      <c r="F36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>marker-add-16x16</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="2" t="s">
+      <c r="J36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="11">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>5.2</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="2" t="str">
+      <c r="C37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="2" t="str">
+      <c r="F37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>zone-edit-16x16</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="2" t="s">
+      <c r="J37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="11">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>5.3</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="2" t="str">
+      <c r="C38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="2" t="str">
+      <c r="F38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>annotation-16x16</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="2" t="s">
+      <c r="J38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="11">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
         <v>5.4</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="2" t="str">
-        <f t="shared" ref="D38" si="6">REPLACE(C38, 1, 2, "")</f>
-        <v>Button</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="C39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="2" t="str">
+        <f t="shared" ref="D39" si="6">REPLACE(C39, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="2" t="str">
-        <f t="shared" ref="F38" si="7">SUBSTITUTE(E38,"_","-")</f>
+      <c r="F39" s="2" t="str">
+        <f t="shared" ref="F39" si="7">SUBSTITUTE(E39,"_","-")</f>
         <v>image-add-16x16</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="2" t="s">
+      <c r="J39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="11">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
         <v>5.5</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="2" t="str">
+      <c r="C40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F39" s="2" t="str">
+      <c r="F40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>image-delete-16x16</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="2" t="s">
+      <c r="J40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="11">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
         <v>5.6</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D40" s="2" t="str">
+      <c r="C41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="2" t="str">
+      <c r="F41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>shading-add-16x16</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="2" t="s">
+      <c r="J41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="10">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
         <v>6</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B42" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="4" t="str">
+      <c r="D42" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-    </row>
-    <row r="42" spans="1:12">
-      <c r="A42" s="11">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
         <v>6.1</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D42" s="2" t="str">
+      <c r="C43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F42" s="2" t="str">
+      <c r="F43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>crossplot-new-16x16</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K42" s="2" t="s">
+      <c r="J43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="11">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
         <v>6.2</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D43" s="2" t="str">
+      <c r="C44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2" t="str">
         <f t="shared" si="5"/>
         <v>Button</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F43" s="2" t="str">
+      <c r="F44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>histogram-new-16x16</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="J44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="10">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
         <v>7</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B45" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="4" t="str">
+      <c r="D45" s="4" t="str">
         <f t="shared" si="5"/>
         <v>Toolbar</v>
       </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="11">
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
         <v>7.1</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Checkbox</v>
-      </c>
-      <c r="F45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="11">
-        <v>7.2</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>138</v>
@@ -2039,15 +2077,15 @@
         <v/>
       </c>
       <c r="G46" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
-        <v>7.3</v>
+        <v>7.2</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>138</v>
@@ -2061,6 +2099,28 @@
         <v/>
       </c>
       <c r="G47" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>Checkbox</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2071,14 +2131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update auto size track dialog
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -869,7 +869,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -880,7 +880,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1005,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" ref="F4:F50" si="0">SUBSTITUTE(E4,"_","-")</f>
+        <f t="shared" ref="F4:F46" si="0">SUBSTITUTE(E4,"_","-")</f>
         <v>save-16x16</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1784,7 +1784,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="4" t="str">
-        <f t="shared" ref="D35:D48" si="5">REPLACE(C35, 1, 2, "")</f>
+        <f t="shared" ref="D35:D44" si="5">REPLACE(C35, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
       <c r="E35" s="5"/>
@@ -2047,14 +2047,14 @@
       <c r="A45" s="10">
         <v>7</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>136</v>
+      <c r="B45" s="15" t="s">
+        <v>147</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D45" s="4" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D45:D46" si="8">REPLACE(C45, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
       <c r="E45" s="5"/>
@@ -2070,117 +2070,117 @@
       <c r="A46" s="11">
         <v>7.1</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>138</v>
+      <c r="B46" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D46" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Checkbox</v>
+        <f t="shared" si="8"/>
+        <v>Button</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>149</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>139</v>
+        <v>auto-size-16x16</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="14" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
-        <v>7.2</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v>Checkbox</v>
-      </c>
-      <c r="F47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="A47" s="10">
+        <v>8</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47" s="4" t="str">
+        <f>REPLACE(C47, 1, 2, "")</f>
+        <v>Toolbar</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
-        <v>7.3</v>
+        <v>8.1</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D48" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f>REPLACE(C48, 1, 2, "")</f>
         <v>Checkbox</v>
       </c>
       <c r="F48" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>SUBSTITUTE(E48,"_","-")</f>
         <v/>
       </c>
       <c r="G48" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="2" t="str">
+        <f>REPLACE(C49, 1, 2, "")</f>
+        <v>Checkbox</v>
+      </c>
+      <c r="F49" s="2" t="str">
+        <f>SUBSTITUTE(E49,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="2" t="str">
+        <f>REPLACE(C50, 1, 2, "")</f>
+        <v>Checkbox</v>
+      </c>
+      <c r="F50" s="2" t="str">
+        <f>SUBSTITUTE(E50,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>8</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D49" s="4" t="str">
-        <f t="shared" ref="D49:D50" si="8">REPLACE(C49, 1, 2, "")</f>
-        <v>Toolbar</v>
-      </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
-        <v>8.1</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v>Button</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>auto-size-16x16</v>
-      </c>
-      <c r="J50" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K50" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add user formular dialog
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="157">
   <si>
     <t>Code</t>
   </si>
@@ -466,13 +466,31 @@
     <t>Databases8Toolbar</t>
   </si>
   <si>
-    <t>AutoSizeTrackCheckbox</t>
-  </si>
-  <si>
     <t>auto_size_16x16</t>
   </si>
   <si>
     <t>Auto Size Track</t>
+  </si>
+  <si>
+    <t>AutoSizeTrackButton</t>
+  </si>
+  <si>
+    <t>TrackBolkUpdateButton</t>
+  </si>
+  <si>
+    <t>CurveBolkUpdateButton</t>
+  </si>
+  <si>
+    <t>track_bolk_16x16</t>
+  </si>
+  <si>
+    <t>Track Bolk Update</t>
+  </si>
+  <si>
+    <t>Curve Bolk Update</t>
+  </si>
+  <si>
+    <t>curve_bolk_16x16</t>
   </si>
 </sst>
 </file>
@@ -869,7 +887,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -877,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1023,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="str">
-        <f t="shared" ref="F4:F46" si="0">SUBSTITUTE(E4,"_","-")</f>
+        <f t="shared" ref="F4:F48" si="0">SUBSTITUTE(E4,"_","-")</f>
         <v>save-16x16</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -2054,7 +2072,7 @@
         <v>13</v>
       </c>
       <c r="D45" s="4" t="str">
-        <f t="shared" ref="D45:D46" si="8">REPLACE(C45, 1, 2, "")</f>
+        <f t="shared" ref="D45:D48" si="8">REPLACE(C45, 1, 2, "")</f>
         <v>Toolbar</v>
       </c>
       <c r="E45" s="5"/>
@@ -2071,7 +2089,7 @@
         <v>7.1</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>15</v>
@@ -2081,7 +2099,7 @@
         <v>Button</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2091,82 +2109,94 @@
         <v>17</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
-        <v>8</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="4" t="str">
-        <f>REPLACE(C47, 1, 2, "")</f>
-        <v>Toolbar</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
+      <c r="A47" s="11">
+        <v>7.2</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Button</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>track-bolk-16x16</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>Button</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="F48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>curve-bolk-16x16</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" s="4" t="str">
+        <f>REPLACE(C49, 1, 2, "")</f>
+        <v>Toolbar</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
         <v>8.1</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" s="2" t="str">
-        <f>REPLACE(C48, 1, 2, "")</f>
-        <v>Checkbox</v>
-      </c>
-      <c r="F48" s="2" t="str">
-        <f>SUBSTITUTE(E48,"_","-")</f>
-        <v/>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="2" t="str">
-        <f>REPLACE(C49, 1, 2, "")</f>
-        <v>Checkbox</v>
-      </c>
-      <c r="F49" s="2" t="str">
-        <f>SUBSTITUTE(E49,"_","-")</f>
-        <v/>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>138</v>
@@ -2180,6 +2210,50 @@
         <v/>
       </c>
       <c r="G50" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="2" t="str">
+        <f>REPLACE(C51, 1, 2, "")</f>
+        <v>Checkbox</v>
+      </c>
+      <c r="F51" s="2" t="str">
+        <f>SUBSTITUTE(E51,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="2" t="str">
+        <f>REPLACE(C52, 1, 2, "")</f>
+        <v>Checkbox</v>
+      </c>
+      <c r="F52" s="2" t="str">
+        <f>SUBSTITUTE(E52,"_","-")</f>
+        <v/>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
duplicate plot, histogram, crossplot data tree
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppServ\www\hoangbd_com\wi-angular\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -88,15 +93,9 @@
     <t>Save as Logplot Template</t>
   </si>
   <si>
-    <t>DuplicateButton</t>
-  </si>
-  <si>
     <t>save_as_16x16</t>
   </si>
   <si>
-    <t>Duplicate Logplot</t>
-  </si>
-  <si>
     <t>PrintButton</t>
   </si>
   <si>
@@ -491,12 +490,18 @@
   </si>
   <si>
     <t>curve_bolk_16x16</t>
+  </si>
+  <si>
+    <t>SaveAsLogplotNameButton</t>
+  </si>
+  <si>
+    <t>Save as Logplot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -887,7 +892,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -897,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1037,8 +1042,8 @@
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
+      <c r="B5" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1048,7 +1053,7 @@
         <v>Button</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1057,8 +1062,8 @@
       <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>24</v>
+      <c r="K5" s="14" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1066,7 +1071,7 @@
         <v>1.4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1076,7 +1081,7 @@
         <v>Button</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1086,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1094,7 +1099,7 @@
         <v>1.5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -1104,7 +1109,7 @@
         <v>Button</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1114,332 +1119,332 @@
         <v>17</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="J8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="G9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="L9" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L15" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L18" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L19" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="L21" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1447,7 +1452,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>13</v>
@@ -1470,7 +1475,7 @@
         <v>2.1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>15</v>
@@ -1480,7 +1485,7 @@
         <v>Button</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F23" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1490,7 +1495,7 @@
         <v>17</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1498,7 +1503,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>15</v>
@@ -1508,7 +1513,7 @@
         <v>Button</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F24" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1518,7 +1523,7 @@
         <v>17</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1526,7 +1531,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>13</v>
@@ -1549,7 +1554,7 @@
         <v>3.1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>15</v>
@@ -1559,7 +1564,7 @@
         <v>Button</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F26" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1569,7 +1574,7 @@
         <v>17</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1577,7 +1582,7 @@
         <v>3.2</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>15</v>
@@ -1587,7 +1592,7 @@
         <v>Button</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F27" s="13" t="str">
         <f t="shared" si="0"/>
@@ -1597,7 +1602,7 @@
         <v>17</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1605,7 +1610,7 @@
         <v>3.3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>15</v>
@@ -1615,7 +1620,7 @@
         <v>Button</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1625,7 +1630,7 @@
         <v>17</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1633,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>13</v>
@@ -1656,7 +1661,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>15</v>
@@ -1666,7 +1671,7 @@
         <v>Button</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F30" s="2" t="str">
         <f>SUBSTITUTE(E30,"_","-")</f>
@@ -1676,7 +1681,7 @@
         <v>17</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1684,7 +1689,7 @@
         <v>4.2</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>15</v>
@@ -1694,7 +1699,7 @@
         <v>Button</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F31" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1704,7 +1709,7 @@
         <v>17</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1712,7 +1717,7 @@
         <v>4.3</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>15</v>
@@ -1722,7 +1727,7 @@
         <v>Button</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F32" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1732,7 +1737,7 @@
         <v>17</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -1740,7 +1745,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>15</v>
@@ -1750,7 +1755,7 @@
         <v>Button</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F33" s="2" t="str">
         <f t="shared" ref="F33" si="4">SUBSTITUTE(E33,"_","-")</f>
@@ -1760,7 +1765,7 @@
         <v>17</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1768,7 +1773,7 @@
         <v>4.5</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>15</v>
@@ -1778,7 +1783,7 @@
         <v>Button</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F34" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1788,7 +1793,7 @@
         <v>17</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -1796,7 +1801,7 @@
         <v>5</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>13</v>
@@ -1819,7 +1824,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>15</v>
@@ -1829,7 +1834,7 @@
         <v>Button</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F36" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1839,7 +1844,7 @@
         <v>17</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1847,7 +1852,7 @@
         <v>5.2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>15</v>
@@ -1857,7 +1862,7 @@
         <v>Button</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F37" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1867,7 +1872,7 @@
         <v>17</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -1875,7 +1880,7 @@
         <v>5.3</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>15</v>
@@ -1885,7 +1890,7 @@
         <v>Button</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F38" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1895,7 +1900,7 @@
         <v>17</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1903,7 +1908,7 @@
         <v>5.4</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>15</v>
@@ -1913,7 +1918,7 @@
         <v>Button</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F39" s="2" t="str">
         <f t="shared" ref="F39" si="7">SUBSTITUTE(E39,"_","-")</f>
@@ -1923,7 +1928,7 @@
         <v>17</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -1931,7 +1936,7 @@
         <v>5.5</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>15</v>
@@ -1941,7 +1946,7 @@
         <v>Button</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F40" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1951,7 +1956,7 @@
         <v>17</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -1959,7 +1964,7 @@
         <v>5.6</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>15</v>
@@ -1969,7 +1974,7 @@
         <v>Button</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F41" s="2" t="str">
         <f t="shared" si="0"/>
@@ -1979,7 +1984,7 @@
         <v>17</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -1987,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>13</v>
@@ -2010,7 +2015,7 @@
         <v>6.1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>15</v>
@@ -2020,7 +2025,7 @@
         <v>Button</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F43" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2030,7 +2035,7 @@
         <v>17</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -2038,7 +2043,7 @@
         <v>6.2</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>15</v>
@@ -2048,7 +2053,7 @@
         <v>Button</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F44" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2058,7 +2063,7 @@
         <v>17</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -2066,7 +2071,7 @@
         <v>7</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>13</v>
@@ -2089,7 +2094,7 @@
         <v>7.1</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>15</v>
@@ -2099,7 +2104,7 @@
         <v>Button</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2109,7 +2114,7 @@
         <v>17</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2117,7 +2122,7 @@
         <v>7.2</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>15</v>
@@ -2127,7 +2132,7 @@
         <v>Button</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2137,7 +2142,7 @@
         <v>17</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2145,7 +2150,7 @@
         <v>7.3</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>15</v>
@@ -2155,7 +2160,7 @@
         <v>Button</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2165,7 +2170,7 @@
         <v>17</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2173,7 +2178,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>13</v>
@@ -2196,10 +2201,10 @@
         <v>8.1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D50" s="2" t="str">
         <f>REPLACE(C50, 1, 2, "")</f>
@@ -2210,7 +2215,7 @@
         <v/>
       </c>
       <c r="G50" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,10 +2223,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D51" s="2" t="str">
         <f>REPLACE(C51, 1, 2, "")</f>
@@ -2232,7 +2237,7 @@
         <v/>
       </c>
       <c r="G51" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2240,10 +2245,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D52" s="2" t="str">
         <f>REPLACE(C52, 1, 2, "")</f>
@@ -2254,7 +2259,7 @@
         <v/>
       </c>
       <c r="G52" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update wi-logplot ui and pre
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\Workspace\Github\wi-angular\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="75" yWindow="1065" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LogPlotTab" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="170">
   <si>
     <t>Code</t>
   </si>
@@ -427,24 +432,12 @@
     <t>Databases7Toolbar</t>
   </si>
   <si>
-    <t>FitWindowCheckbox</t>
-  </si>
-  <si>
-    <t>wiCheckbox</t>
-  </si>
-  <si>
     <t>Fit Window</t>
   </si>
   <si>
-    <t>ReferenceLineCheckbox</t>
-  </si>
-  <si>
     <t>Reference Line</t>
   </si>
   <si>
-    <t>TooltipCheckbox</t>
-  </si>
-  <si>
     <t>Tool tip</t>
   </si>
   <si>
@@ -491,12 +484,63 @@
   </si>
   <si>
     <t>CurveBulkUpdateButton</t>
+  </si>
+  <si>
+    <t>Databases9Toolbar</t>
+  </si>
+  <si>
+    <t>EditCurveButton</t>
+  </si>
+  <si>
+    <t>BaselineShiftButton</t>
+  </si>
+  <si>
+    <t>DepthShiftButton</t>
+  </si>
+  <si>
+    <t>curve_depth_shift_16x16</t>
+  </si>
+  <si>
+    <t>Edit Curve</t>
+  </si>
+  <si>
+    <t>Baseline Shift</t>
+  </si>
+  <si>
+    <t>Depth Shift</t>
+  </si>
+  <si>
+    <t>curve_edit_16x16</t>
+  </si>
+  <si>
+    <t>curve_interactive_baseline_edit_16x16</t>
+  </si>
+  <si>
+    <t>is-check-type</t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>wiLogplot.getwiD3Ctrl().referenceLine()</t>
+  </si>
+  <si>
+    <t>wiLogplot.getwiD3Ctrl().tooltip()</t>
+  </si>
+  <si>
+    <t>FitWindowButton</t>
+  </si>
+  <si>
+    <t>ReferenceLineButton</t>
+  </si>
+  <si>
+    <t>TooltipButton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -551,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +626,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -887,7 +935,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -895,28 +943,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="59" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="10.375" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.75" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="40.875" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.875" style="2" customWidth="1"/>
     <col min="8" max="9" width="11" style="2"/>
     <col min="10" max="10" width="13.5" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11" style="2"/>
+    <col min="12" max="13" width="11" style="2"/>
+    <col min="14" max="14" width="46.25" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -953,8 +1002,14 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -977,7 +1032,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
@@ -1005,7 +1060,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>1.2</v>
       </c>
@@ -1033,12 +1088,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>1.3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1058,10 +1113,10 @@
         <v>17</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" s="6">
         <v>1.4</v>
       </c>
@@ -1089,7 +1144,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" s="6">
         <v>1.5</v>
       </c>
@@ -1117,7 +1172,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -1143,7 +1198,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1166,7 +1221,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1189,7 +1244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1212,7 +1267,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
@@ -1235,7 +1290,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1258,7 +1313,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
@@ -1281,7 +1336,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1304,7 +1359,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1327,7 +1382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -1350,7 +1405,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>66</v>
       </c>
@@ -1373,7 +1428,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
@@ -1396,7 +1451,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -1419,12 +1474,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>15</v>
@@ -1433,7 +1488,7 @@
         <v>38</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>40</v>
@@ -1442,7 +1497,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" s="10">
         <v>2</v>
       </c>
@@ -1465,7 +1520,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" s="11">
         <v>2.1</v>
       </c>
@@ -1493,7 +1548,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" s="11">
         <v>2.2000000000000002</v>
       </c>
@@ -1521,7 +1576,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" s="10">
         <v>3</v>
       </c>
@@ -1544,7 +1599,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="11">
         <v>3.1</v>
       </c>
@@ -1572,7 +1627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A27" s="12">
         <v>3.2</v>
       </c>
@@ -1600,7 +1655,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" s="11">
         <v>3.3</v>
       </c>
@@ -1628,7 +1683,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1651,7 +1706,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" s="11">
         <v>4.0999999999999996</v>
       </c>
@@ -1679,7 +1734,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" s="11">
         <v>4.2</v>
       </c>
@@ -1707,7 +1762,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" s="11">
         <v>4.3</v>
       </c>
@@ -1735,7 +1790,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" s="11">
         <v>4.4000000000000004</v>
       </c>
@@ -1763,7 +1818,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="11">
         <v>4.5</v>
       </c>
@@ -1791,7 +1846,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="10">
         <v>5</v>
       </c>
@@ -1814,7 +1869,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A36" s="11">
         <v>5.0999999999999996</v>
       </c>
@@ -1842,7 +1897,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" s="11">
         <v>5.2</v>
       </c>
@@ -1870,7 +1925,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A38" s="11">
         <v>5.3</v>
       </c>
@@ -1898,7 +1953,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A39" s="11">
         <v>5.4</v>
       </c>
@@ -1926,7 +1981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A40" s="11">
         <v>5.5</v>
       </c>
@@ -1954,7 +2009,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A41" s="11">
         <v>5.6</v>
       </c>
@@ -1982,7 +2037,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A42" s="10">
         <v>6</v>
       </c>
@@ -2005,7 +2060,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A43" s="11">
         <v>6.1</v>
       </c>
@@ -2033,7 +2088,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A44" s="11">
         <v>6.2</v>
       </c>
@@ -2061,12 +2116,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" s="10">
         <v>7</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>13</v>
@@ -2084,12 +2139,12 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A46" s="11">
         <v>7.1</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>15</v>
@@ -2099,7 +2154,7 @@
         <v>Button</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2109,15 +2164,15 @@
         <v>17</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A47" s="11">
         <v>7.2</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>15</v>
@@ -2127,7 +2182,7 @@
         <v>Button</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2137,15 +2192,15 @@
         <v>17</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A48" s="11">
         <v>7.3</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>15</v>
@@ -2155,7 +2210,7 @@
         <v>Button</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2165,15 +2220,15 @@
         <v>17</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A49" s="10">
         <v>8</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>134</v>
+      <c r="B49" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>13</v>
@@ -2191,70 +2246,204 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A50" s="11">
         <v>8.1</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>136</v>
+      <c r="B50" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D50" s="2" t="str">
         <f>REPLACE(C50, 1, 2, "")</f>
-        <v>Checkbox</v>
+        <v>Button</v>
       </c>
       <c r="F50" s="2" t="str">
         <f>SUBSTITUTE(E50,"_","-")</f>
         <v/>
       </c>
       <c r="G50" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M50" s="2">
+        <v>1</v>
+      </c>
+      <c r="N50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A51" s="11">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>136</v>
+      <c r="B51" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D51" s="2" t="str">
         <f>REPLACE(C51, 1, 2, "")</f>
-        <v>Checkbox</v>
+        <v>Button</v>
       </c>
       <c r="F51" s="2" t="str">
         <f>SUBSTITUTE(E51,"_","-")</f>
         <v/>
       </c>
       <c r="G51" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M51" s="2">
+        <v>1</v>
+      </c>
+      <c r="N51" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A52" s="11">
         <v>8.3000000000000007</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>136</v>
+      <c r="B52" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>15</v>
       </c>
       <c r="D52" s="2" t="str">
         <f>REPLACE(C52, 1, 2, "")</f>
-        <v>Checkbox</v>
+        <v>Button</v>
       </c>
       <c r="F52" s="2" t="str">
         <f>SUBSTITUTE(E52,"_","-")</f>
         <v/>
       </c>
       <c r="G52" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="M52" s="2">
+        <v>1</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A53" s="16">
+        <v>9</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53" s="17" t="str">
+        <f>REPLACE(C53, 1, 2, "")</f>
+        <v>Toolbar</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A54" s="11">
+        <v>9.1</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="14" t="str">
+        <f>REPLACE(C54, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="F54" s="2" t="str">
+        <f t="shared" ref="F54:F56" si="9">SUBSTITUTE(E54,"_","-")</f>
+        <v>curve-edit-16x16</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A55" s="11">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="14" t="str">
+        <f>REPLACE(C55, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F55" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>curve-interactive-baseline-edit-16x16</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A56" s="11">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="14" t="str">
+        <f>REPLACE(C56, 1, 2, "")</f>
+        <v>Button</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F56" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>curve-depth-shift-16x16</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="14" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2460,7 @@
       <selection sqref="A1:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Horizontal Adjustment update & fix table log track properties
</commit_message>
<xml_diff>
--- a/Wi-LogPlot.Nam.xlsx
+++ b/Wi-LogPlot.Nam.xlsx
@@ -427,9 +427,6 @@
     <t>Databases7Toolbar</t>
   </si>
   <si>
-    <t>Fit Window</t>
-  </si>
-  <si>
     <t>Reference Line</t>
   </si>
   <si>
@@ -533,6 +530,9 @@
   </si>
   <si>
     <t>wiLogplot.getwiD3Ctrl().fitWindow()</t>
+  </si>
+  <si>
+    <t>Horizontal Adjustment</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -943,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="59" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="N47" sqref="N47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="59" zoomScaleNormal="85" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1001,10 +1001,10 @@
         <v>11</v>
       </c>
       <c r="M1" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="N1" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1091,7 +1091,7 @@
         <v>1.3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1111,7 +1111,7 @@
         <v>17</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1474,10 +1474,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>139</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>15</v>
@@ -1486,7 +1486,7 @@
         <v>38</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>40</v>
@@ -2142,7 +2142,7 @@
         <v>7.1</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>15</v>
@@ -2152,7 +2152,7 @@
         <v>Button</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F46" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2162,7 +2162,7 @@
         <v>17</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
         <v>7.2</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>15</v>
@@ -2180,7 +2180,7 @@
         <v>Button</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F47" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2190,7 +2190,7 @@
         <v>17</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -2198,7 +2198,7 @@
         <v>7.3</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>15</v>
@@ -2208,7 +2208,7 @@
         <v>Button</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F48" s="2" t="str">
         <f t="shared" si="0"/>
@@ -2218,7 +2218,7 @@
         <v>17</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
@@ -2226,7 +2226,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>13</v>
@@ -2249,7 +2249,7 @@
         <v>8.1</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>15</v>
@@ -2262,8 +2262,8 @@
         <f>SUBSTITUTE(E50,"_","-")</f>
         <v/>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>135</v>
+      <c r="G50" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>40</v>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="N50" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>15</v>
@@ -2297,7 +2297,7 @@
         <v/>
       </c>
       <c r="G51" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H51" s="14" t="s">
         <v>40</v>
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="N51" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -2317,7 +2317,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>15</v>
@@ -2331,7 +2331,7 @@
         <v/>
       </c>
       <c r="G52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>40</v>
@@ -2343,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>13</v>
@@ -2374,7 +2374,7 @@
         <v>9.1</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>15</v>
@@ -2384,7 +2384,7 @@
         <v>Button</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F54" s="2" t="str">
         <f t="shared" ref="F54:F56" si="10">SUBSTITUTE(E54,"_","-")</f>
@@ -2394,7 +2394,7 @@
         <v>17</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
@@ -2402,7 +2402,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>15</v>
@@ -2412,7 +2412,7 @@
         <v>Button</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F55" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2422,7 +2422,7 @@
         <v>17</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>15</v>
@@ -2440,7 +2440,7 @@
         <v>Button</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F56" s="2" t="str">
         <f t="shared" si="10"/>
@@ -2450,7 +2450,7 @@
         <v>17</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>